<commit_message>
Add Message Entity Update Databasemodell for group chat
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="128">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -382,13 +382,34 @@
   </si>
   <si>
     <t>pictureURI</t>
+  </si>
+  <si>
+    <t>messageID</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>NOT NULL; UNSIGNED; UNIQUE</t>
+  </si>
+  <si>
+    <t>NOT NULL; UNSIGNED;</t>
+  </si>
+  <si>
+    <t>Messages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +446,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -619,7 +646,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -653,6 +680,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -5199,6 +5227,358 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="de-DE" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>306916</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Straight Arrow Connector 68"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2931583" y="9196916"/>
+          <a:ext cx="10584" cy="2360084"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="TextBox 70"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3111500" y="9154583"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>148166</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="TextBox 71"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3069167" y="11197166"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>931333</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Arrow Connector 72"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4582583" y="9239250"/>
+          <a:ext cx="21167" cy="2307167"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>52917</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="808567" cy="287841"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="TextBox 75"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4667250" y="9196917"/>
+          <a:ext cx="808567" cy="287841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>groupID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>52917</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Curved Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7545917" y="8413750"/>
+          <a:ext cx="3630083" cy="3450167"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 57580"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31749</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="808567" cy="287841"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="TextBox 91"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7545916" y="11853334"/>
+          <a:ext cx="808567" cy="287841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>userID</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5793,10 +6173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AD57"/>
+  <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6917,6 +7297,115 @@
         <v>67</v>
       </c>
     </row>
+    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B61" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B62" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" s="29"/>
+    </row>
+    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B64" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10" t="str">
+        <f>D44</f>
+        <v>MEDIUMINT</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10" t="str">
+        <f>P41</f>
+        <v>MEDIUMINT</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" s="15"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" s="15"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G67" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Database Modell Make Thread safe ...
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -351,9 +351,6 @@
     <t>profilePictureURI</t>
   </si>
   <si>
-    <t>phoneNrHash</t>
-  </si>
-  <si>
     <t>bqID</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>Messages</t>
+  </si>
+  <si>
+    <t>phoneNumberHash</t>
   </si>
 </sst>
 </file>
@@ -6176,7 +6176,7 @@
   <dimension ref="B3:AD67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:E67"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6202,7 +6202,7 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N3" s="30" t="s">
         <v>102</v>
@@ -6248,7 +6248,7 @@
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>33</v>
@@ -6264,7 +6264,7 @@
       </c>
       <c r="G5" s="29"/>
       <c r="N5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>33</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="str">
@@ -6388,7 +6388,7 @@
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>54</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>58</v>
@@ -6568,7 +6568,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="6"/>
       <c r="N17" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="18" t="str">
@@ -6688,14 +6688,14 @@
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="20" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",E21)),"X","")</f>
@@ -6705,7 +6705,7 @@
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N26" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.25">
@@ -6733,7 +6733,7 @@
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N28" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O28" s="10" t="s">
         <v>33</v>
@@ -6922,10 +6922,10 @@
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="O42" s="10"/>
       <c r="P42" s="10" t="s">
@@ -7009,7 +7009,7 @@
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>33</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N53" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y53" s="5" t="s">
         <v>96</v>
@@ -7237,7 +7237,7 @@
     </row>
     <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N55" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O55" s="10" t="s">
         <v>33</v>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="2:30" x14ac:dyDescent="0.25">
@@ -7324,7 +7324,7 @@
     </row>
     <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>33</v>
@@ -7333,7 +7333,7 @@
         <v>56</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>33</v>
@@ -7342,7 +7342,7 @@
     </row>
     <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B64" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="str">
@@ -7350,7 +7350,7 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>33</v>
@@ -7367,7 +7367,7 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>33</v>
@@ -7376,11 +7376,11 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>39</v>
@@ -7392,7 +7392,7 @@
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="20" t="s">

</xml_diff>

<commit_message>
update Database Modell make some things better
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="119">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -171,9 +171,6 @@
     <t>score</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>VARCHAR(30)</t>
   </si>
   <si>
@@ -252,18 +249,6 @@
     <t>rightAnswerID</t>
   </si>
   <si>
-    <t>doubedRightAnswer</t>
-  </si>
-  <si>
-    <t>NOT NUL; DEFAULT: false</t>
-  </si>
-  <si>
-    <t>doubed</t>
-  </si>
-  <si>
-    <t>NOT NULL; DEFUALT false</t>
-  </si>
-  <si>
     <t>additionalInformation</t>
   </si>
   <si>
@@ -327,9 +312,6 @@
     <t>datatype</t>
   </si>
   <si>
-    <t>Winners</t>
-  </si>
-  <si>
     <t>Answers</t>
   </si>
   <si>
@@ -351,18 +333,6 @@
     <t>profilePictureURI</t>
   </si>
   <si>
-    <t>bqID</t>
-  </si>
-  <si>
-    <t>isBet</t>
-  </si>
-  <si>
-    <t>NOT NULL;</t>
-  </si>
-  <si>
-    <t>BQs</t>
-  </si>
-  <si>
     <t>groupID</t>
   </si>
   <si>
@@ -372,15 +342,9 @@
     <t>GroupsToUsers</t>
   </si>
   <si>
-    <t>BQsToUsers</t>
-  </si>
-  <si>
     <t>sumOfUsersToAnswer</t>
   </si>
   <si>
-    <t>pictureURI</t>
-  </si>
-  <si>
     <t>messageID</t>
   </si>
   <si>
@@ -403,6 +367,15 @@
   </si>
   <si>
     <t>phoneNumberHash</t>
+  </si>
+  <si>
+    <t>questionID</t>
+  </si>
+  <si>
+    <t>questionsToUsers</t>
+  </si>
+  <si>
+    <t>Questions</t>
   </si>
 </sst>
 </file>
@@ -1806,9 +1779,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>137583</xdr:rowOff>
+      <xdr:colOff>658091</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -1823,12 +1796,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7059083" y="3947583"/>
-          <a:ext cx="4127500" cy="973667"/>
+          <a:off x="7013864" y="3550227"/>
+          <a:ext cx="4127500" cy="1371023"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj1" fmla="val -140"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -2059,7 +2032,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1139562</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
@@ -2110,13 +2083,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>878416</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>74083</xdr:rowOff>
+      <xdr:colOff>885826</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>885826</xdr:colOff>
+      <xdr:colOff>891886</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -2126,9 +2099,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3503083" y="4074583"/>
-          <a:ext cx="7410" cy="3831167"/>
+        <a:xfrm flipH="1">
+          <a:off x="3509531" y="3532909"/>
+          <a:ext cx="6060" cy="4372841"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2206,9 +2179,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>934245</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>41009</xdr:rowOff>
+      <xdr:colOff>977541</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>32350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -2218,7 +2191,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3558912" y="4041509"/>
+          <a:off x="3601246" y="3461350"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2905,31 +2878,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>488156</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>83344</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Elbow Connector 17"/>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7465219" y="750094"/>
-          <a:ext cx="3429000" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 25640"/>
-          </a:avLst>
+        <a:xfrm flipH="1">
+          <a:off x="22288500" y="3548062"/>
+          <a:ext cx="1" cy="1563688"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln w="38100">
           <a:headEnd type="triangle"/>
@@ -2953,23 +2924,171 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>236084</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>51708</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="22203115" y="5869781"/>
+          <a:ext cx="2041" cy="1611427"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="17386300" y="8248650"/>
+          <a:ext cx="2863850" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="285990"/>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>321469</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="TextBox 38"/>
+        <xdr:cNvPr id="44" name="TextBox 43"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7422356" y="666750"/>
-          <a:ext cx="400050" cy="285990"/>
+          <a:off x="20019169" y="8253413"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>33074</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>145521</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="TextBox 44"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17273324" y="8337021"/>
+          <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3007,21 +3126,125 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>226218</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>407458</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>83345</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvPr id="46" name="TextBox 45"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10632281" y="369094"/>
+          <a:off x="22463125" y="5798345"/>
           <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>488157</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>97897</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="TextBox 46"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22543824" y="4669897"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6614</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="321469" cy="259797"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="TextBox 48"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22516042" y="3435614"/>
+          <a:ext cx="321469" cy="259797"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3057,166 +3280,22 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="22288500" y="3548062"/>
-          <a:ext cx="1" cy="1563688"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>236084</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>154781</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>51708</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="22203115" y="5869781"/>
-          <a:ext cx="2041" cy="1611427"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="Straight Arrow Connector 42"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="17386300" y="8248650"/>
-          <a:ext cx="2863850" cy="6350"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>321469</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:colOff>480219</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="TextBox 43"/>
+        <xdr:cNvPr id="50" name="TextBox 49"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20019169" y="8253413"/>
+          <a:off x="22535886" y="7227094"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3255,270 +3334,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>33074</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>145521</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="TextBox 44"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17273324" y="8337021"/>
-          <a:ext cx="400050" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>407458</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>83345</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="TextBox 45"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22463125" y="5798345"/>
-          <a:ext cx="400050" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>488157</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>97897</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="TextBox 46"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22543824" y="4669897"/>
-          <a:ext cx="400050" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>460375</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6614</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="321469" cy="259797"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="TextBox 48"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22516042" y="3435614"/>
-          <a:ext cx="321469" cy="259797"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>480219</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="TextBox 49"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22535886" y="7227094"/>
-          <a:ext cx="400050" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>364142</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>16819</xdr:rowOff>
+      <xdr:colOff>390119</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>120728</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2398107" cy="1097075"/>
     <xdr:sp macro="" textlink="">
@@ -3528,7 +3347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="364142" y="4588819"/>
+          <a:off x="390119" y="3740228"/>
           <a:ext cx="2398107" cy="1097075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3627,27 +3446,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>124872</xdr:rowOff>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:colOff>649432</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>131233</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="21" name="Straight Arrow Connector 20"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="53" idx="1"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4270375" y="4125372"/>
-          <a:ext cx="53975" cy="3816361"/>
+          <a:off x="4273262" y="3515591"/>
+          <a:ext cx="30306" cy="4426142"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3676,9 +3493,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>173567</xdr:rowOff>
+      <xdr:colOff>699077</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>17703</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1037166" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -3688,7 +3505,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4324350" y="3983567"/>
+          <a:off x="4353213" y="3446703"/>
           <a:ext cx="1037166" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3727,21 +3544,21 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>96309</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="645582" cy="283609"/>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>583141</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>29634</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="607483" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="TextBox 53"/>
+        <xdr:cNvPr id="60" name="TextBox 59"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10585450" y="1048809"/>
-          <a:ext cx="645582" cy="283609"/>
+          <a:off x="10527241" y="3268134"/>
+          <a:ext cx="607483" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3779,20 +3596,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>583141</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>29634</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>20109</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>185209</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="607483" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="TextBox 59"/>
+        <xdr:cNvPr id="67" name="TextBox 66"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10527241" y="3268134"/>
+          <a:off x="10573809" y="5519209"/>
           <a:ext cx="607483" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3831,58 +3648,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>20109</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>185209</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="607483" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="TextBox 66"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10573809" y="5519209"/>
-          <a:ext cx="607483" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>bqID</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1144058</xdr:colOff>
       <xdr:row>43</xdr:row>
@@ -4284,162 +4049,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>148168</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>306919</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="124" name="Elbow Connector 123"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="16920106" y="5878512"/>
-          <a:ext cx="2261658" cy="1468969"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 99696"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>52915</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>42334</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>296336</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>10586</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="133" name="Elbow Connector 132"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="15716250" y="2434166"/>
-          <a:ext cx="4730752" cy="1471087"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 112"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>814917</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="624416" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="140" name="TextBox 139"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17272000" y="804333"/>
-          <a:ext cx="624416" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>userID</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>232834</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>116417</xdr:rowOff>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>485780</xdr:colOff>
+      <xdr:colOff>485782</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>152403</xdr:rowOff>
     </xdr:to>
@@ -4450,12 +4067,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6593417" y="4116917"/>
-          <a:ext cx="4475696" cy="1369486"/>
+          <a:off x="6511637" y="3550227"/>
+          <a:ext cx="4512259" cy="1936176"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 99421"/>
+            <a:gd name="adj1" fmla="val 99894"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -4534,9 +4151,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>776816</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:colOff>811452</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>32712</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -4546,7 +4163,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7137399" y="3894667"/>
+          <a:off x="7167225" y="3461712"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4684,9 +4301,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1788583</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
+      <xdr:colOff>1749137</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>77932</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -4701,12 +4318,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5439833" y="4296833"/>
-          <a:ext cx="5715000" cy="3399367"/>
+          <a:off x="5403273" y="3506932"/>
+          <a:ext cx="5706341" cy="4189268"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 370"/>
+            <a:gd name="adj1" fmla="val -228"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -4733,9 +4350,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1890183</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>1803592</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>178955</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="607483" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -4745,7 +4362,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5541433" y="4032250"/>
+          <a:off x="5457728" y="3417455"/>
           <a:ext cx="607483" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4853,55 +4470,6 @@
         <a:xfrm rot="10800000">
           <a:off x="7572377" y="8972551"/>
           <a:ext cx="3524248" cy="1285875"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="186" name="Elbow Connector 185"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7581900" y="1057274"/>
-          <a:ext cx="3467100" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6086,7 +5654,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="2"/>
       <c r="L20" s="2" t="s">
@@ -6175,8 +5743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6202,10 +5770,7 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -6227,28 +5792,10 @@
       <c r="G4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="27" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>33</v>
@@ -6257,76 +5804,41 @@
         <v>43</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="29"/>
-      <c r="N5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="12" t="str">
-        <f>D5</f>
-        <v>INT</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="29"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="13" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="15"/>
-      <c r="N6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="11" t="str">
-        <f>P29</f>
-        <v>MEDIUMINT</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="21"/>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>33</v>
+      <c r="E7" s="13"/>
+      <c r="F7" s="10" t="str">
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E7)),"*","")</f>
+        <v/>
       </c>
       <c r="G7" s="15"/>
       <c r="O7" s="10"/>
@@ -6337,135 +5849,143 @@
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="13"/>
+      <c r="D8" s="10" t="str">
+        <f>P41</f>
+        <v>MEDIUMINT</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="F8" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E8)),"*","")</f>
-        <v/>
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E8)),"X","")</f>
+        <v>X</v>
       </c>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="str">
-        <f>P41</f>
+        <f>D44</f>
         <v>MEDIUMINT</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E9)),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G9" s="15"/>
+        <f t="shared" ref="F9" si="0">IF(ISNUMBER(SEARCH("NOT NULL",E9)),"X","")</f>
+        <v/>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="10" t="str">
-        <f>D44</f>
-        <v>MEDIUMINT</v>
+      <c r="D10" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="10" t="str">
-        <f t="shared" ref="F10" si="0">IF(ISNUMBER(SEARCH("NOT NULL",E10)),"X","")</f>
+        <v>39</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="str">
+        <f t="shared" ref="F11:F14" si="1">IF(ISNUMBER(SEARCH("NOT NULL",E11)),"X","")</f>
         <v/>
-      </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="F12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>X</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="10" t="str">
-        <f t="shared" ref="F13:F16" si="1">IF(ISNUMBER(SEARCH("NOT NULL",E13)),"X","")</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>X</v>
       </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F14" s="10" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y14" s="30" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>38</v>
+      <c r="B15" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F15" s="13"/>
       <c r="G15" s="6"/>
       <c r="N15" s="17" t="s">
         <v>40</v>
@@ -6505,25 +6025,25 @@
       </c>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>83</v>
+      <c r="B16" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="F16" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E16)),"X","")</f>
         <v>X</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>66</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O16" s="18" t="s">
         <v>33</v>
@@ -6532,14 +6052,14 @@
         <v>43</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="S16" s="19"/>
       <c r="Y16" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="Z16" s="12" t="s">
         <v>33</v>
@@ -6548,7 +6068,7 @@
         <v>43</v>
       </c>
       <c r="AB16" s="28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AC16" s="12" t="s">
         <v>33</v>
@@ -6556,19 +6076,26 @@
       <c r="AD16" s="29"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="6"/>
+      <c r="B17" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="str">
+        <f>P16</f>
+        <v>INT</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="11" t="str">
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E17)),"X","")</f>
+        <v/>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="N17" s="18" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="18" t="str">
@@ -6583,7 +6110,7 @@
       </c>
       <c r="S17" s="19"/>
       <c r="Y17" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="Z17" s="10" t="s">
         <v>33</v>
@@ -6601,29 +6128,12 @@
       <c r="AD17" s="15"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E18)),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="N18" s="18" t="s">
         <v>47</v>
       </c>
       <c r="O18" s="18"/>
       <c r="P18" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q18" s="19" t="s">
         <v>39</v>
@@ -6633,11 +6143,11 @@
       </c>
       <c r="S18" s="19"/>
       <c r="Y18" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Z18" s="11"/>
       <c r="AA18" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB18" s="20" t="s">
         <v>39</v>
@@ -6647,61 +6157,21 @@
       </c>
       <c r="AD18" s="21"/>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="str">
-        <f>P16</f>
-        <v>INT</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E19)),"X","")</f>
-        <v/>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="B20" s="10"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E20)),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="20" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E21)),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G21" s="8"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N26" s="26" t="s">
@@ -6728,12 +6198,12 @@
         <v>5</v>
       </c>
       <c r="Y27" s="16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N28" s="5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="O28" s="10" t="s">
         <v>33</v>
@@ -6787,7 +6257,7 @@
       </c>
       <c r="S29" s="15"/>
       <c r="Y29" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="Z29" s="12" t="s">
         <v>33</v>
@@ -6796,7 +6266,7 @@
         <v>43</v>
       </c>
       <c r="AB29" s="28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AC29" s="12" t="s">
         <v>33</v>
@@ -6804,28 +6274,28 @@
       <c r="AD29" s="29"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N30" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10" t="str">
+      <c r="N30" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11" t="str">
         <f>P16</f>
         <v>INT</v>
       </c>
-      <c r="Q30" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="R30" s="10"/>
-      <c r="S30" s="6"/>
+      <c r="Q30" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="8"/>
       <c r="T30" s="13"/>
       <c r="Y30" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="Z30" s="11" t="s">
         <v>33</v>
       </c>
       <c r="AA30" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AB30" s="11" t="s">
         <v>39</v>
@@ -6836,20 +6306,12 @@
       <c r="AD30" s="21"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N31" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q31" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="R31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="S31" s="8"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
       <c r="Z31" s="10"/>
       <c r="AA31" s="10"/>
       <c r="AB31" s="13"/>
@@ -6858,7 +6320,7 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N39" s="16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
@@ -6881,7 +6343,7 @@
         <v>5</v>
       </c>
       <c r="Y40" s="26" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
@@ -6892,10 +6354,10 @@
         <v>33</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q41" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R41" s="12" t="s">
         <v>33</v>
@@ -6922,17 +6384,17 @@
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N42" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="O42" s="10"/>
       <c r="P42" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q42" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R42" s="10" t="s">
         <v>33</v>
@@ -6976,11 +6438,11 @@
         <v>5</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O43" s="10"/>
       <c r="P43" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q43" s="10" t="s">
         <v>39</v>
@@ -6990,7 +6452,7 @@
       </c>
       <c r="S43" s="15"/>
       <c r="Y43" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="Z43" s="11" t="s">
         <v>33</v>
@@ -7009,23 +6471,23 @@
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G44" s="29"/>
       <c r="N44" s="25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="O44" s="10"/>
       <c r="P44" s="10" t="s">
@@ -7046,7 +6508,7 @@
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
@@ -7060,11 +6522,11 @@
       </c>
       <c r="G45" s="6"/>
       <c r="N45" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="O45" s="10"/>
       <c r="P45" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q45" s="10"/>
       <c r="R45" s="10"/>
@@ -7072,7 +6534,7 @@
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="str">
@@ -7087,29 +6549,29 @@
       </c>
       <c r="G46" s="15"/>
       <c r="N46" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="O46" s="11"/>
       <c r="P46" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q46" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R46" s="11" t="s">
         <v>33</v>
       </c>
       <c r="S46" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>39</v>
@@ -7121,11 +6583,11 @@
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -7141,7 +6603,7 @@
     </row>
     <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y50" s="31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="2:30" x14ac:dyDescent="0.25">
@@ -7166,16 +6628,16 @@
     </row>
     <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y52" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Z52" s="10" t="s">
         <v>33</v>
       </c>
       <c r="AA52" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="AB52" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC52" s="10" t="s">
         <v>33</v>
@@ -7184,14 +6646,14 @@
     </row>
     <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N53" s="26" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="Y53" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="Z53" s="10"/>
       <c r="AA53" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB53" s="13" t="s">
         <v>39</v>
@@ -7221,11 +6683,11 @@
         <v>5</v>
       </c>
       <c r="Y54" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="Z54" s="11"/>
       <c r="AA54" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB54" s="20" t="s">
         <v>39</v>
@@ -7237,7 +6699,7 @@
     </row>
     <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N55" s="5" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="O55" s="10" t="s">
         <v>33</v>
@@ -7285,21 +6747,21 @@
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q57" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R57" s="11" t="s">
         <v>33</v>
       </c>
       <c r="S57" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="2:30" x14ac:dyDescent="0.25">
@@ -7324,16 +6786,16 @@
     </row>
     <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>33</v>
@@ -7342,7 +6804,7 @@
     </row>
     <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B64" s="25" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="str">
@@ -7350,7 +6812,7 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>33</v>
@@ -7367,7 +6829,7 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>33</v>
@@ -7376,11 +6838,11 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="33" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>39</v>
@@ -7392,7 +6854,7 @@
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="20" t="s">
@@ -7425,7 +6887,7 @@
   <sheetData>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="31" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -7439,23 +6901,23 @@
         <v>35</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>

</xml_diff>

<commit_message>
Modify Database Modell Add SQL Statements
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="123">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Messages</t>
   </si>
   <si>
-    <t>phoneNumberHash</t>
-  </si>
-  <si>
     <t>questionID</t>
   </si>
   <si>
@@ -376,6 +373,21 @@
   </si>
   <si>
     <t>Questions</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>VARCHAR(2)</t>
+  </si>
+  <si>
+    <t>UNSIGNED;</t>
+  </si>
+  <si>
+    <t>passwordhash</t>
+  </si>
+  <si>
+    <t>VARCHAR(25)</t>
   </si>
 </sst>
 </file>
@@ -3545,20 +3557,20 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>583141</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>29634</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="607483" cy="283609"/>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>185209</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1020499" cy="279135"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="TextBox 59"/>
+        <xdr:cNvPr id="67" name="TextBox 66"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10527241" y="3268134"/>
-          <a:ext cx="607483" cy="283609"/>
+          <a:off x="10156031" y="5519209"/>
+          <a:ext cx="1020499" cy="279135"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3587,59 +3599,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>bqID</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>20109</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>185209</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="607483" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="TextBox 66"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10573809" y="5519209"/>
-          <a:ext cx="607483" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>bqID</a:t>
+            <a:t>questionID</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5146,6 +5106,58 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1400" b="1"/>
             <a:t>userID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>107157</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1020499" cy="279135"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="TextBox 69"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10048876" y="3333750"/>
+          <a:ext cx="1020499" cy="279135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>questionID</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5743,8 +5755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5770,7 +5782,7 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -5794,22 +5806,22 @@
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -5979,6 +5991,7 @@
       <c r="B15" s="25" t="s">
         <v>107</v>
       </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
         <v>57</v>
       </c>
@@ -6076,26 +6089,26 @@
       <c r="AD16" s="29"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11" t="str">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="str">
         <f>P16</f>
         <v>INT</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="11" t="str">
+      <c r="F17" s="10" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",E17)),"X","")</f>
         <v/>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>66</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="18" t="str">
@@ -6128,6 +6141,21 @@
       <c r="AD17" s="15"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="20" t="str">
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E18)),"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="G18" s="8"/>
       <c r="N18" s="18" t="s">
         <v>47</v>
       </c>
@@ -6175,7 +6203,7 @@
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N26" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.25">
@@ -6203,7 +6231,7 @@
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N28" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O28" s="10" t="s">
         <v>33</v>
@@ -6347,22 +6375,22 @@
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N41" s="3" t="s">
+      <c r="N41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="O41" s="12" t="s">
+      <c r="O41" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="P41" s="12" t="s">
+      <c r="P41" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Q41" s="28" t="s">
+      <c r="Q41" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="R41" s="12" t="s">
+      <c r="R41" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S41" s="29"/>
+      <c r="S41" s="15"/>
       <c r="Y41" s="27" t="s">
         <v>40</v>
       </c>
@@ -6387,15 +6415,13 @@
         <v>105</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="O42" s="10"/>
       <c r="P42" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q42" s="13" t="s">
-        <v>71</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="Q42" s="13"/>
       <c r="R42" s="10" t="s">
         <v>33</v>
       </c>
@@ -6442,10 +6468,10 @@
       </c>
       <c r="O43" s="10"/>
       <c r="P43" s="10" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="Q43" s="10" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="R43" s="10" t="s">
         <v>33</v>
@@ -6548,20 +6574,20 @@
         <v>33</v>
       </c>
       <c r="G46" s="15"/>
-      <c r="N46" s="7" t="s">
+      <c r="N46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11" t="s">
+      <c r="O46" s="10"/>
+      <c r="P46" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="Q46" s="11" t="s">
+      <c r="Q46" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="R46" s="11" t="s">
+      <c r="R46" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S46" s="8" t="s">
+      <c r="S46" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6580,6 +6606,20 @@
         <v>33</v>
       </c>
       <c r="G47" s="15"/>
+      <c r="N47" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O47" s="11"/>
+      <c r="P47" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q47" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R47" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="8"/>
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
@@ -6829,7 +6869,7 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F65" s="13" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Update SQL and Modell
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="124">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -5758,8 +5758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P48" sqref="P48"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5872,11 +5872,11 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",E8)),"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
       <c r="G8" s="15"/>
     </row>
@@ -6883,9 +6883,7 @@
       <c r="E65" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F65" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="F65" s="13"/>
       <c r="G65" s="15"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Databasemodell; Update SQL; Impement UserCreation to TestUtil; Add some methods to TestUtil
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="128">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Wettgruppen</t>
   </si>
   <si>
-    <t>rightAnswerID</t>
-  </si>
-  <si>
     <t>additionalInformation</t>
   </si>
   <si>
@@ -391,6 +388,21 @@
   </si>
   <si>
     <t>pictureURI</t>
+  </si>
+  <si>
+    <t>phoneNumberHash</t>
+  </si>
+  <si>
+    <t>selectedAnswerID</t>
+  </si>
+  <si>
+    <t>contactID</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -2145,16 +2157,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1547813</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>607219</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1549400</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>631031</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2162,9 +2174,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15406688" y="9032875"/>
-          <a:ext cx="1587" cy="1003300"/>
+        <a:xfrm flipH="1">
+          <a:off x="13430250" y="9167812"/>
+          <a:ext cx="23812" cy="2643188"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2401,9 +2413,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>518319</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>149226</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>40746</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
@@ -2414,7 +2426,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6876257" y="9375246"/>
+          <a:off x="7662070" y="8994246"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2454,9 +2466,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>305065</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:colOff>293158</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -2466,7 +2478,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10888398" y="10366375"/>
+          <a:off x="10842096" y="12461874"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2505,62 +2517,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1667934</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>20108</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="400050" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="TextBox 33"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15553267" y="9735608"/>
-          <a:ext cx="400050" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1668199</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>739513</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>67581</xdr:rowOff>
+      <xdr:rowOff>186643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="400050" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -2570,7 +2530,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15527074" y="9021081"/>
+          <a:off x="13562544" y="9140143"/>
           <a:ext cx="400050" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2843,16 +2803,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>391584</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>582084</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
+      <xdr:colOff>488156</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2861,12 +2821,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6752167" y="9228667"/>
-          <a:ext cx="4413250" cy="1481666"/>
+          <a:off x="7608094" y="8977312"/>
+          <a:ext cx="3429000" cy="3393282"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -120"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -3664,9 +3624,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>162984</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>48684</xdr:rowOff>
+      <xdr:colOff>424921</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>120122</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="963083" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -3676,7 +3636,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10107084" y="9954684"/>
+          <a:off x="10366640" y="11740622"/>
           <a:ext cx="963083" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3715,16 +3675,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>940594</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>952501</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>169334</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>137586</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3732,9 +3692,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="13009563" y="9048750"/>
-          <a:ext cx="10584" cy="994836"/>
+        <a:xfrm flipV="1">
+          <a:off x="12096750" y="9179718"/>
+          <a:ext cx="11907" cy="2345532"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3760,22 +3720,69 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>211667</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="Straight Arrow Connector 102"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13091584" y="5958416"/>
+          <a:ext cx="10583" cy="1471083"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>201084</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>10583</xdr:rowOff>
+      <xdr:colOff>275166</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179916</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="624416" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="TextBox 101"/>
+        <xdr:cNvPr id="106" name="TextBox 105"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13081001" y="9726083"/>
+          <a:off x="13155083" y="7037916"/>
           <a:ext cx="624416" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3815,105 +3822,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>211667</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>52916</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="103" name="Straight Arrow Connector 102"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="13091584" y="5958416"/>
-          <a:ext cx="10583" cy="1471083"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>275166</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>179916</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="624416" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="TextBox 105"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13155083" y="7037916"/>
-          <a:ext cx="624416" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>userID</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
       <xdr:colOff>232833</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -4414,15 +4322,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:colOff>535781</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4431,12 +4339,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="7572377" y="8972551"/>
-          <a:ext cx="3524248" cy="1285875"/>
+          <a:off x="7572375" y="8763002"/>
+          <a:ext cx="3512344" cy="3333749"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 33390"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="28575">
@@ -5161,6 +5069,363 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1400" b="1"/>
             <a:t>questionID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>679716</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>8202</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="TextBox 74"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13502747" y="11438202"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1046428</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>82020</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="624416" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="TextBox 76"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12202584" y="11321520"/>
+          <a:ext cx="624416" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>userID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>334434</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>127263</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="TextBox 78"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20003559" y="11366763"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>785813</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>595316</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>119064</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Elbow Connector 84"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="17192626" y="9060656"/>
+          <a:ext cx="3071815" cy="3059908"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>488156</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="624416" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="TextBox 90"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19550062" y="12180094"/>
+          <a:ext cx="624416" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>userID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>511968</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="Straight Arrow Connector 92"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16918781" y="9191625"/>
+          <a:ext cx="3250406" cy="2655094"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>178593</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="400050" cy="283609"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="TextBox 94"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16585406" y="9227344"/>
+          <a:ext cx="400050" cy="283609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5758,8 +6023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="K24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5785,7 +6050,7 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -5810,7 +6075,7 @@
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>33</v>
@@ -5844,7 +6109,7 @@
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
@@ -5882,7 +6147,7 @@
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="str">
@@ -5900,7 +6165,7 @@
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>53</v>
@@ -5909,7 +6174,7 @@
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
@@ -5925,7 +6190,7 @@
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
@@ -5940,7 +6205,7 @@
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
@@ -5959,7 +6224,7 @@
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
@@ -5974,15 +6239,15 @@
       </c>
       <c r="G14" s="6"/>
       <c r="N14" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y14" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
@@ -6037,7 +6302,7 @@
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
@@ -6065,7 +6330,7 @@
       </c>
       <c r="S16" s="19"/>
       <c r="Y16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z16" s="12" t="s">
         <v>33</v>
@@ -6074,7 +6339,7 @@
         <v>43</v>
       </c>
       <c r="AB16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC16" s="12" t="s">
         <v>33</v>
@@ -6100,7 +6365,7 @@
         <v>66</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="18" t="str">
@@ -6115,7 +6380,7 @@
       </c>
       <c r="S17" s="19"/>
       <c r="Y17" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z17" s="10" t="s">
         <v>33</v>
@@ -6134,7 +6399,7 @@
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="str">
@@ -6166,7 +6431,7 @@
       </c>
       <c r="S18" s="19"/>
       <c r="Y18" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z18" s="11"/>
       <c r="AA18" s="20" t="s">
@@ -6182,11 +6447,11 @@
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>39</v>
@@ -6215,7 +6480,7 @@
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N26" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.25">
@@ -6238,12 +6503,12 @@
         <v>5</v>
       </c>
       <c r="Y27" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N28" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O28" s="10" t="s">
         <v>33</v>
@@ -6297,7 +6562,7 @@
       </c>
       <c r="S29" s="15"/>
       <c r="Y29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z29" s="12" t="s">
         <v>33</v>
@@ -6306,7 +6571,7 @@
         <v>43</v>
       </c>
       <c r="AB29" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC29" s="12" t="s">
         <v>33</v>
@@ -6329,13 +6594,13 @@
       <c r="S30" s="8"/>
       <c r="T30" s="13"/>
       <c r="Y30" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z30" s="11" t="s">
         <v>33</v>
       </c>
       <c r="AA30" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB30" s="11" t="s">
         <v>39</v>
@@ -6360,7 +6625,7 @@
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N39" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
@@ -6383,7 +6648,7 @@
         <v>5</v>
       </c>
       <c r="Y40" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
@@ -6424,16 +6689,18 @@
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O42" s="10"/>
       <c r="P42" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q42" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="Q42" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="R42" s="10" t="s">
         <v>33</v>
       </c>
@@ -6476,21 +6743,17 @@
         <v>5</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q43" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="R43" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S43" s="15"/>
+        <v>123</v>
+      </c>
+      <c r="P43" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>127</v>
+      </c>
+      <c r="S43" s="6"/>
       <c r="Y43" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z43" s="11" t="s">
         <v>33</v>
@@ -6509,7 +6772,7 @@
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>33</v>
@@ -6524,20 +6787,20 @@
         <v>33</v>
       </c>
       <c r="G44" s="29"/>
-      <c r="N44" s="25" t="s">
-        <v>83</v>
+      <c r="N44" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="O44" s="10"/>
       <c r="P44" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q44" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="R44" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q44" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="R44" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S44" s="6"/>
+      <c r="S44" s="15"/>
       <c r="Z44" s="10"/>
       <c r="AA44" s="10"/>
       <c r="AB44" s="13"/>
@@ -6546,7 +6809,7 @@
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
@@ -6560,14 +6823,18 @@
       </c>
       <c r="G45" s="6"/>
       <c r="N45" s="25" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="O45" s="10"/>
       <c r="P45" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="Q45" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R45" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="S45" s="6"/>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
@@ -6586,22 +6853,16 @@
         <v>33</v>
       </c>
       <c r="G46" s="15"/>
-      <c r="N46" s="5" t="s">
-        <v>79</v>
+      <c r="N46" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="O46" s="10"/>
       <c r="P46" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S46" s="6" t="s">
-        <v>66</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="6"/>
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
@@ -6618,24 +6879,26 @@
         <v>33</v>
       </c>
       <c r="G47" s="15"/>
-      <c r="N47" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="O47" s="11"/>
-      <c r="P47" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q47" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="R47" s="20" t="s">
+      <c r="N47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q47" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="R47" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S47" s="8"/>
+      <c r="S47" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="20" t="s">
@@ -6644,6 +6907,20 @@
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="8"/>
+      <c r="N48" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q48" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R48" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="S48" s="8"/>
     </row>
     <row r="49" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B49" s="13"/>
@@ -6655,7 +6932,7 @@
     </row>
     <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y50" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="2:30" x14ac:dyDescent="0.25">
@@ -6680,13 +6957,13 @@
     </row>
     <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y52" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z52" s="10" t="s">
         <v>33</v>
       </c>
       <c r="AA52" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB52" s="10" t="s">
         <v>71</v>
@@ -6697,11 +6974,8 @@
       <c r="AD52" s="15"/>
     </row>
     <row r="53" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N53" s="26" t="s">
-        <v>106</v>
-      </c>
       <c r="Y53" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Z53" s="10"/>
       <c r="AA53" s="10" t="s">
@@ -6716,26 +6990,8 @@
       <c r="AD53" s="15"/>
     </row>
     <row r="54" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N54" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="O54" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="P54" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q54" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="R54" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="S54" s="23" t="s">
-        <v>5</v>
-      </c>
       <c r="Y54" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z54" s="11"/>
       <c r="AA54" s="11" t="s">
@@ -6750,23 +7006,6 @@
       <c r="AD54" s="21"/>
     </row>
     <row r="55" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N55" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O55" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P55" s="10" t="str">
-        <f>D44</f>
-        <v>MEDIUMINT</v>
-      </c>
-      <c r="Q55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R55" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S55" s="15"/>
       <c r="Y55" s="10"/>
       <c r="Z55" s="10"/>
       <c r="AA55" s="10"/>
@@ -6774,46 +7013,9 @@
       <c r="AC55" s="10"/>
       <c r="AD55" s="13"/>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N56" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="O56" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P56" s="10" t="str">
-        <f>P41</f>
-        <v>MEDIUMINT</v>
-      </c>
-      <c r="Q56" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="R56" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S56" s="15"/>
-    </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N57" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q57" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R57" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="S57" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="61" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="2:30" x14ac:dyDescent="0.25">
@@ -6835,10 +7037,16 @@
       <c r="G62" s="23" t="s">
         <v>5</v>
       </c>
+      <c r="N62" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y62" s="16" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="63" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>33</v>
@@ -6847,16 +7055,52 @@
         <v>55</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G63" s="29"/>
+      <c r="N63" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O63" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="P63" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q63" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="R63" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S63" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y63" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z63" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA63" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB63" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC63" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD63" s="23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B64" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="str">
@@ -6864,14 +7108,48 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G64" s="6"/>
+      <c r="N64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P64" s="10">
+        <f>D53</f>
+        <v>0</v>
+      </c>
+      <c r="Q64" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S64" s="15"/>
+      <c r="Y64" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA64" s="10" t="str">
+        <f>P41</f>
+        <v>MEDIUMINT</v>
+      </c>
+      <c r="AB64" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD64" s="15"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>48</v>
       </c>
@@ -6881,18 +7159,52 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F65" s="13"/>
       <c r="G65" s="15"/>
+      <c r="N65" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P65" s="10">
+        <f>P50</f>
+        <v>0</v>
+      </c>
+      <c r="Q65" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="R65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S65" s="15"/>
+      <c r="Y65" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z65" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA65" s="11" t="str">
+        <f>P41</f>
+        <v>MEDIUMINT</v>
+      </c>
+      <c r="AB65" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC65" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD65" s="21"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>39</v>
@@ -6901,10 +7213,32 @@
         <v>33</v>
       </c>
       <c r="G66" s="15"/>
+      <c r="N66" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q66" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="R66" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S66" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y66" s="10"/>
+      <c r="Z66" s="10"/>
+      <c r="AA66" s="10"/>
+      <c r="AB66" s="10"/>
+      <c r="AC66" s="10"/>
+      <c r="AD66" s="10"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="20" t="s">
@@ -6937,7 +7271,7 @@
   <sheetData>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -6951,23 +7285,23 @@
         <v>35</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>

</xml_diff>

<commit_message>
Edit and Add Documents
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -6023,8 +6023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update SQL and Modell; Add Abläufe; Update Trigger; Update Codes
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modell Fabi" sheetId="1" r:id="rId1"/>
@@ -393,9 +393,6 @@
     <t>PublicQuestions</t>
   </si>
   <si>
-    <t>AnswersOfPrivateQuestions</t>
-  </si>
-  <si>
     <t>PrivateQuestionsToUsers</t>
   </si>
   <si>
@@ -441,10 +438,13 @@
     <t>Notifications.notificationD</t>
   </si>
   <si>
-    <t>AnswersOfPublicQuestions</t>
-  </si>
-  <si>
     <t>AnswersOfPublicQuestionss.answerID</t>
+  </si>
+  <si>
+    <t>AnswersPublicQuestions</t>
+  </si>
+  <si>
+    <t>AnswersPrivateQuestions</t>
   </si>
 </sst>
 </file>
@@ -5000,8 +5000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5053,7 +5053,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>40</v>
@@ -5071,7 +5071,7 @@
         <v>32</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Y4" s="22" t="s">
         <v>40</v>
@@ -5089,7 +5089,7 @@
         <v>32</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
@@ -5126,7 +5126,7 @@
       </c>
       <c r="S5" s="29"/>
       <c r="Y5" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Z5" s="10" t="s">
         <v>33</v>
@@ -5172,7 +5172,7 @@
         <v>33</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>42</v>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y7" s="5" t="s">
         <v>74</v>
@@ -5249,7 +5249,7 @@
         <v/>
       </c>
       <c r="G8" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>104</v>
@@ -5281,7 +5281,7 @@
         <v/>
       </c>
       <c r="AD8" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
@@ -5301,7 +5301,7 @@
         <v/>
       </c>
       <c r="G9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>105</v>
@@ -5539,7 +5539,7 @@
         <v/>
       </c>
       <c r="G17" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N17" s="16" t="s">
         <v>100</v>
@@ -5577,12 +5577,12 @@
         <v>32</v>
       </c>
       <c r="S18" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="20" t="s">
@@ -5651,7 +5651,7 @@
         <v>33</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y21" s="16" t="s">
         <v>140</v>
@@ -5688,7 +5688,7 @@
         <v>32</v>
       </c>
       <c r="AD22" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
@@ -5735,7 +5735,7 @@
         <v>33</v>
       </c>
       <c r="AD24" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
@@ -5756,7 +5756,7 @@
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
@@ -5776,7 +5776,7 @@
         <v>32</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
@@ -5814,7 +5814,7 @@
         <v>33</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N31" s="26" t="s">
         <v>101</v>
@@ -5851,7 +5851,7 @@
         <v>32</v>
       </c>
       <c r="S32" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.25">
@@ -5872,7 +5872,7 @@
         <v>33</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.25">
@@ -5893,10 +5893,10 @@
         <v>33</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y34" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.25">
@@ -5930,7 +5930,7 @@
         <v>32</v>
       </c>
       <c r="AD35" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.25">
@@ -5951,7 +5951,7 @@
         <v>33</v>
       </c>
       <c r="AD36" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.25">
@@ -5972,7 +5972,7 @@
         <v>33</v>
       </c>
       <c r="AD37" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.25">
@@ -5989,12 +5989,12 @@
       </c>
       <c r="AC38" s="11"/>
       <c r="AD38" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
@@ -6014,7 +6014,7 @@
         <v>32</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
@@ -6035,7 +6035,7 @@
         <v>33</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
@@ -6056,7 +6056,7 @@
         <v>33</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N44" s="16" t="s">
         <v>93</v>
@@ -6096,7 +6096,7 @@
         <v>32</v>
       </c>
       <c r="S45" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
@@ -6181,7 +6181,7 @@
         <v>32</v>
       </c>
       <c r="AD49" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="2:30" x14ac:dyDescent="0.25">
@@ -6262,14 +6262,14 @@
     </row>
     <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N53" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11" t="s">
         <v>57</v>
       </c>
       <c r="Q53" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R53" s="11" t="s">
         <v>33</v>
@@ -6298,7 +6298,7 @@
         <v>32</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="2:30" x14ac:dyDescent="0.25">
@@ -6319,7 +6319,7 @@
         <v>33</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y59" s="30" t="s">
         <v>94</v>
@@ -6343,7 +6343,7 @@
         <v>33</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y60" s="27" t="s">
         <v>40</v>
@@ -6361,7 +6361,7 @@
         <v>32</v>
       </c>
       <c r="AD60" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="2:30" x14ac:dyDescent="0.25">
@@ -6402,7 +6402,7 @@
         <v>32</v>
       </c>
       <c r="S62" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Y62" s="5" t="s">
         <v>80</v>
@@ -6421,7 +6421,7 @@
         <v>33</v>
       </c>
       <c r="AD62" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="2:30" x14ac:dyDescent="0.25">
@@ -6442,7 +6442,7 @@
         <v>33</v>
       </c>
       <c r="S63" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Y63" s="7" t="s">
         <v>85</v>
@@ -6477,7 +6477,7 @@
         <v>33</v>
       </c>
       <c r="S64" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="2:22" x14ac:dyDescent="0.25">
@@ -6502,7 +6502,7 @@
         <v>32</v>
       </c>
       <c r="G72" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Entities, Insert Add/Create methods to query interface;
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -725,13 +725,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
-    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
-    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
-    <cellStyle name="Bad" xfId="5" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Akzent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Akzent3" xfId="6" builtinId="37"/>
+    <cellStyle name="Akzent4" xfId="4" builtinId="41"/>
+    <cellStyle name="Akzent6" xfId="3" builtinId="49"/>
+    <cellStyle name="Schlecht" xfId="5" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Zelle überprüfen" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4705,7 +4705,7 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -5000,11 +5000,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y61" sqref="Y61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
@@ -6584,7 +6584,7 @@
       <selection activeCell="D8" sqref="D8:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="31" t="s">

</xml_diff>

<commit_message>
Update SQL; Test for Trigger; working on implementation of querymanager; working on the SQLFactory; add some methods to Util; Update databaseModell;
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="143">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>AnswersPrivateQuestions</t>
+  </si>
+  <si>
+    <t>UNSIGEND; NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -725,13 +728,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Akzent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Akzent3" xfId="6" builtinId="37"/>
-    <cellStyle name="Akzent4" xfId="4" builtinId="41"/>
-    <cellStyle name="Akzent6" xfId="3" builtinId="49"/>
-    <cellStyle name="Schlecht" xfId="5" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Zelle überprüfen" xfId="1" builtinId="23"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2240,9 +2243,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>302078</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>157843</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="276225" cy="283609"/>
     <xdr:sp macro="" textlink="">
@@ -2252,7 +2255,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2714625" y="3600450"/>
+          <a:off x="2778578" y="3586843"/>
           <a:ext cx="276225" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2443,14 +2446,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47632</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2279203</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>95252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>500742</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -2461,8 +2464,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="5938842" y="5414967"/>
-          <a:ext cx="4381498" cy="600068"/>
+          <a:off x="7030135" y="5413606"/>
+          <a:ext cx="4381498" cy="602789"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -4705,7 +4708,7 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -5000,11 +5003,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y61" sqref="Y61"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
@@ -5093,22 +5096,22 @@
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="15"/>
+      <c r="F5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="29"/>
       <c r="N5" s="3" t="s">
         <v>103</v>
       </c>
@@ -5125,22 +5128,22 @@
         <v>33</v>
       </c>
       <c r="S5" s="29"/>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Z5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA5" s="10" t="s">
+      <c r="Z5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AB5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD5" s="15"/>
+      <c r="AC5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD5" s="29"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -5430,16 +5433,16 @@
       </c>
       <c r="G13" s="6"/>
       <c r="Y13" s="25" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="Z13" s="10"/>
-      <c r="AA13" s="10" t="s">
-        <v>38</v>
+      <c r="AA13" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="AB13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC13" s="10" t="str">
+        <v>39</v>
+      </c>
+      <c r="AC13" s="13" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",AB13)),"X","")</f>
         <v>X</v>
       </c>
@@ -5464,16 +5467,16 @@
         <v>65</v>
       </c>
       <c r="Y14" s="24" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="Z14" s="11"/>
-      <c r="AA14" s="20" t="s">
-        <v>112</v>
+      <c r="AA14" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="AB14" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC14" s="20" t="str">
+        <v>66</v>
+      </c>
+      <c r="AC14" s="11" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",AB14)),"X","")</f>
         <v>X</v>
       </c>
@@ -5492,25 +5495,19 @@
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="6"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>38</v>
+      <c r="D16" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="10" t="str">
+        <v>39</v>
+      </c>
+      <c r="F16" s="13" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",E16)),"X","")</f>
         <v>X</v>
       </c>
@@ -5524,43 +5521,43 @@
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="13" t="str">
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E17)),"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="N17" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="str">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="str">
         <f>D30</f>
         <v>INT</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="10" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E17)),"X","")</f>
+      <c r="F18" s="10" t="str">
+        <f>IF(ISNUMBER(SEARCH("NOT NULL",E18)),"X","")</f>
         <v/>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="N17" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="13" t="str">
-        <f>IF(ISNUMBER(SEARCH("NOT NULL",E18)),"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G18" s="6"/>
       <c r="N18" s="22" t="s">
         <v>40</v>
       </c>
@@ -5582,16 +5579,16 @@
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="C19" s="11"/>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="20" t="str">
+        <v>66</v>
+      </c>
+      <c r="F19" s="11" t="str">
         <f>IF(ISNUMBER(SEARCH("NOT NULL",E19)),"X","")</f>
         <v>X</v>
       </c>
@@ -5985,7 +5982,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="20" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="AC38" s="11"/>
       <c r="AD38" s="8" t="s">
@@ -6584,7 +6581,7 @@
       <selection activeCell="D8" sqref="D8:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="31" t="s">

</xml_diff>

<commit_message>
Different Changes Update SQLFactory Add Entities Update Model Update QueryManager
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="132">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -261,24 +261,6 @@
     <t>accessionDate</t>
   </si>
   <si>
-    <t>notificationID</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>VARCHAR(3)</t>
-  </si>
-  <si>
-    <t>NOT NULL; UNSIGNED; AUTO_INCREMENT</t>
-  </si>
-  <si>
-    <t>parameterID</t>
-  </si>
-  <si>
-    <t>parameterText</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -303,15 +285,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>NotificationsParameters</t>
-  </si>
-  <si>
-    <t>Notifications</t>
-  </si>
-  <si>
-    <t>NotificationsToUsers</t>
-  </si>
-  <si>
     <t>groupPictureURI</t>
   </si>
   <si>
@@ -429,15 +402,9 @@
     <t>NOT NULL; DEFAULT:0</t>
   </si>
   <si>
-    <t>Notification.notificationID</t>
-  </si>
-  <si>
     <t>PublicQuestions.questionID</t>
   </si>
   <si>
-    <t>Notifications.notificationD</t>
-  </si>
-  <si>
     <t>AnswersOfPublicQuestionss.answerID</t>
   </si>
   <si>
@@ -448,9 +415,6 @@
   </si>
   <si>
     <t>UNSIGEND; NOT NULL</t>
-  </si>
-  <si>
-    <t>parameterDescription</t>
   </si>
 </sst>
 </file>
@@ -502,7 +466,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,11 +490,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
@@ -540,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -671,30 +630,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -722,20 +667,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Accent3" xfId="6" builtinId="37"/>
-    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
+    <cellStyle name="Accent3" xfId="5" builtinId="37"/>
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
-    <cellStyle name="Bad" xfId="5" builtinId="27"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3309,26 +3251,26 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123826</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="65" name="Straight Arrow Connector 64"/>
+        <xdr:cNvPr id="70" name="Straight Arrow Connector 69"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12915900" y="10163175"/>
-          <a:ext cx="9526" cy="1428750"/>
+        <a:xfrm flipH="1">
+          <a:off x="22440900" y="2714625"/>
+          <a:ext cx="1" cy="1276350"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3355,22 +3297,118 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>466728</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Elbow Connector 72"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="18011777" y="4238627"/>
+          <a:ext cx="4276724" cy="638172"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 99889"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Straight Arrow Connector 74"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19831050" y="6667500"/>
+          <a:ext cx="657225" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="276225" cy="283609"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="68" name="TextBox 67"/>
+        <xdr:cNvPr id="82" name="TextBox 81"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13001625" y="11306175"/>
+          <a:off x="20288250" y="6334125"/>
           <a:ext cx="276225" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3409,254 +3447,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="69" name="TextBox 68"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12973050" y="10058400"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="70" name="Straight Arrow Connector 69"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="22440900" y="2714625"/>
-          <a:ext cx="1" cy="1276350"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>466728</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Elbow Connector 72"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="18011777" y="4238627"/>
-          <a:ext cx="4276724" cy="638172"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 99889"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Straight Arrow Connector 74"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19831050" y="6667500"/>
-          <a:ext cx="657225" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="82" name="TextBox 81"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20288250" y="6334125"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>10</xdr:row>
@@ -3671,310 +3461,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="20259675" y="2028825"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>285751</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Straight Arrow Connector 85"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="22564726" y="9734550"/>
-          <a:ext cx="9524" cy="1485900"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="88" name="TextBox 87"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22593300" y="10896600"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="89" name="TextBox 88"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="22593300" y="9686925"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="90" name="Straight Arrow Connector 89"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="17611726" y="9496425"/>
-          <a:ext cx="2933699" cy="2514600"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="91" name="TextBox 90"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17554575" y="11563350"/>
-          <a:ext cx="276225" cy="283609"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="276225" cy="283609"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="TextBox 91"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20345400" y="9239250"/>
           <a:ext cx="276225" cy="283609"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5006,8 +4492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC63" sqref="AC63"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5033,13 +4519,13 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -5059,7 +4545,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>40</v>
@@ -5077,7 +4563,7 @@
         <v>32</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="Y4" s="22" t="s">
         <v>40</v>
@@ -5095,12 +4581,12 @@
         <v>32</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>33</v>
@@ -5108,15 +4594,15 @@
       <c r="D5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>58</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="28"/>
       <c r="N5" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>33</v>
@@ -5124,15 +4610,15 @@
       <c r="P5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="28" t="s">
-        <v>107</v>
+      <c r="Q5" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="R5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="29"/>
+      <c r="S5" s="28"/>
       <c r="Y5" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="Z5" s="12" t="s">
         <v>33</v>
@@ -5140,13 +4626,13 @@
       <c r="AA5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="28" t="s">
+      <c r="AB5" s="27" t="s">
         <v>58</v>
       </c>
       <c r="AC5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AD5" s="29"/>
+      <c r="AD5" s="28"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -5164,7 +4650,7 @@
       </c>
       <c r="G6" s="15"/>
       <c r="N6" s="25" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10" t="str">
@@ -5172,13 +4658,13 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>33</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>42</v>
@@ -5218,11 +4704,11 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="Y7" s="5" t="s">
         <v>74</v>
@@ -5255,14 +4741,14 @@
         <v/>
       </c>
       <c r="G8" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="O8" s="10"/>
-      <c r="P8" s="33" t="s">
-        <v>106</v>
+      <c r="P8" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="Q8" s="13" t="s">
         <v>39</v>
@@ -5275,9 +4761,9 @@
         <v>41</v>
       </c>
       <c r="Z8" s="10"/>
-      <c r="AA8" s="10" t="str">
+      <c r="AA8" s="10">
         <f>Q62</f>
-        <v>Einschränkungen</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="13" t="s">
         <v>45</v>
@@ -5287,12 +4773,12 @@
         <v/>
       </c>
       <c r="AD8" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="str">
@@ -5307,10 +4793,10 @@
         <v/>
       </c>
       <c r="G9" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="20" t="s">
@@ -5324,7 +4810,7 @@
       </c>
       <c r="S9" s="8"/>
       <c r="Y9" s="5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="Z9" s="10"/>
       <c r="AA9" s="13" t="s">
@@ -5336,7 +4822,7 @@
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="13" t="s">
@@ -5436,11 +4922,11 @@
       </c>
       <c r="G13" s="6"/>
       <c r="Y13" s="25" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Z13" s="10"/>
       <c r="AA13" s="13" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="AB13" s="13" t="s">
         <v>39</v>
@@ -5487,7 +4973,7 @@
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
@@ -5501,11 +4987,11 @@
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>39</v>
@@ -5524,7 +5010,7 @@
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13" t="s">
@@ -5539,12 +5025,12 @@
       </c>
       <c r="G17" s="6"/>
       <c r="N17" s="16" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="str">
@@ -5559,7 +5045,7 @@
         <v/>
       </c>
       <c r="G18" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>40</v>
@@ -5577,7 +5063,7 @@
         <v>32</v>
       </c>
       <c r="S18" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
@@ -5597,7 +5083,7 @@
       </c>
       <c r="G19" s="8"/>
       <c r="N19" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>33</v>
@@ -5605,13 +5091,13 @@
       <c r="P19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Q19" s="28" t="s">
+      <c r="Q19" s="27" t="s">
         <v>59</v>
       </c>
       <c r="R19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S19" s="29"/>
+      <c r="S19" s="28"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N20" s="25" t="s">
@@ -5651,10 +5137,10 @@
         <v>33</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="Y21" s="16" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
@@ -5688,12 +5174,12 @@
         <v>32</v>
       </c>
       <c r="AD22" s="17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N23" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="20" t="s">
@@ -5721,7 +5207,7 @@
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y24" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18" t="str">
@@ -5735,7 +5221,7 @@
         <v>33</v>
       </c>
       <c r="AD24" s="19" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
@@ -5756,7 +5242,7 @@
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
@@ -5776,7 +5262,7 @@
         <v>32</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
@@ -5800,7 +5286,7 @@
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="str">
@@ -5814,10 +5300,10 @@
         <v>33</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.25">
@@ -5851,12 +5337,12 @@
         <v>32</v>
       </c>
       <c r="S32" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N33" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="O33" s="10" t="s">
         <v>33</v>
@@ -5872,7 +5358,7 @@
         <v>33</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.25">
@@ -5893,10 +5379,10 @@
         <v>33</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="Y34" s="26" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.25">
@@ -5930,12 +5416,12 @@
         <v>32</v>
       </c>
       <c r="AD35" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y36" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="Z36" s="10" t="s">
         <v>33</v>
@@ -5951,7 +5437,7 @@
         <v>33</v>
       </c>
       <c r="AD36" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.25">
@@ -5972,7 +5458,7 @@
         <v>33</v>
       </c>
       <c r="AD37" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.25">
@@ -5985,16 +5471,16 @@
         <v>0</v>
       </c>
       <c r="AB38" s="20" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="AC38" s="11"/>
       <c r="AD38" s="8" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
@@ -6014,12 +5500,12 @@
         <v>32</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>33</v>
@@ -6035,7 +5521,7 @@
         <v>33</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
@@ -6056,7 +5542,7 @@
         <v>33</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
@@ -6073,10 +5559,10 @@
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="N44" s="16" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
@@ -6096,7 +5582,7 @@
         <v>32</v>
       </c>
       <c r="S45" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
@@ -6109,17 +5595,17 @@
       <c r="P46" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Q46" s="28" t="s">
+      <c r="Q46" s="27" t="s">
         <v>63</v>
       </c>
       <c r="R46" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S46" s="29"/>
+      <c r="S46" s="28"/>
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N47" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="O47" s="10"/>
       <c r="P47" s="10" t="s">
@@ -6135,28 +5621,25 @@
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N48" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="O48" s="10"/>
       <c r="P48" s="13" t="s">
         <v>53</v>
       </c>
       <c r="Q48" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="R48" s="10"/>
       <c r="S48" s="6"/>
-      <c r="Y48" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N49" s="5" t="s">
         <v>69</v>
       </c>
       <c r="O49" s="10"/>
       <c r="P49" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="Q49" s="10" t="s">
         <v>70</v>
@@ -6165,26 +5648,8 @@
         <v>33</v>
       </c>
       <c r="S49" s="15"/>
-      <c r="Y49" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z49" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA49" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB49" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC49" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD49" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N50" s="25" t="s">
         <v>79</v>
       </c>
@@ -6199,26 +5664,10 @@
         <v>33</v>
       </c>
       <c r="S50" s="6"/>
-      <c r="Y50" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z50" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA50" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB50" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC50" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD50" s="29"/>
-    </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N51" s="25" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="O51" s="10"/>
       <c r="P51" s="10" t="s">
@@ -6227,30 +5676,14 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
       <c r="S51" s="6"/>
-      <c r="Y51" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z51" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA51" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB51" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC51" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD51" s="21"/>
-    </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N52" s="25" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="O52" s="10"/>
       <c r="P52" s="13" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="Q52" s="13" t="s">
         <v>39</v>
@@ -6260,28 +5693,28 @@
       </c>
       <c r="S52" s="6"/>
     </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N53" s="24" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11" t="s">
         <v>57</v>
       </c>
       <c r="Q53" s="11" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="R53" s="11" t="s">
         <v>33</v>
       </c>
       <c r="S53" s="8"/>
     </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58" s="22" t="s">
         <v>40</v>
       </c>
@@ -6298,10 +5731,10 @@
         <v>32</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>48</v>
       </c>
@@ -6313,21 +5746,18 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y59" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>33</v>
@@ -6343,160 +5773,12 @@
         <v>33</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y60" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z60" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA60" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB60" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC60" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD60" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N61" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y61" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B71" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="Z61" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA61" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB61" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC61" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD61" s="29"/>
-    </row>
-    <row r="62" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N62" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="O62" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P62" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q62" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="R62" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="S62" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y62" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z62" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA62" s="10" t="str">
-        <f>AA50</f>
-        <v>INT</v>
-      </c>
-      <c r="AB62" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC62" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD62" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N63" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O63" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="P63" s="12" t="str">
-        <f>P46</f>
-        <v>MEDIUMINT</v>
-      </c>
-      <c r="Q63" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="R63" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="S63" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y63" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z63" s="10"/>
-      <c r="AA63" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB63" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC63" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD63" s="6"/>
-    </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N64" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O64" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P64" s="11" t="str">
-        <f>AA50</f>
-        <v>INT</v>
-      </c>
-      <c r="Q64" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R64" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="S64" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y64" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z64" s="11"/>
-      <c r="AA64" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB64" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC64" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD64" s="21"/>
-    </row>
-    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B71" s="31" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="72" spans="2:22" x14ac:dyDescent="0.25">
@@ -6516,18 +5798,18 @@
         <v>32</v>
       </c>
       <c r="G72" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>70</v>
@@ -6539,7 +5821,7 @@
     </row>
     <row r="74" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
@@ -6555,7 +5837,7 @@
     </row>
     <row r="75" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
@@ -6601,8 +5883,8 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="31" t="s">
-        <v>91</v>
+      <c r="D8" s="29" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -6615,24 +5897,24 @@
       <c r="F9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>89</v>
+      <c r="G9" s="30" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>

</xml_diff>

<commit_message>
add reset password and lots more
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="134">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>UNSIGEND; NOT NULL</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>VARCHAR()</t>
   </si>
 </sst>
 </file>
@@ -3601,7 +3607,7 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>1592035</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="276225" cy="283609"/>
@@ -4492,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U72" sqref="U72"/>
+    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q57" sqref="Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5614,100 +5620,110 @@
       <c r="Q47" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="R47" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="R47" s="10"/>
       <c r="S47" s="15"/>
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="N48" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="O48" s="10"/>
+      <c r="N48" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="O48">
+        <v>100</v>
+      </c>
       <c r="P48" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q48" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="R48" s="10"/>
+        <v>133</v>
+      </c>
       <c r="S48" s="6"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N49" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O49" s="10"/>
+      <c r="P49" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q49" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="R49" s="10"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N50" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q49" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="R49" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S49" s="15"/>
-    </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="N50" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="O50" s="10"/>
       <c r="P50" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q50" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="R50" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="S50" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="Q50" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="R50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S50" s="15"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N51" s="25" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="O51" s="10"/>
       <c r="P51" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="Q51" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R51" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="S51" s="6"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N52" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="6"/>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N53" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="O52" s="10"/>
-      <c r="P52" s="13" t="s">
+      <c r="O53" s="10"/>
+      <c r="P53" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="Q52" s="13" t="s">
+      <c r="Q53" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="R52" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="S52" s="6"/>
-    </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="N53" s="24" t="s">
+      <c r="R53" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N54" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11" t="s">
+      <c r="O54" s="11"/>
+      <c r="P54" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="Q53" s="11" t="s">
+      <c r="Q54" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="R53" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="S53" s="8"/>
+      <c r="R54" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S54" s="8"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">

</xml_diff>

<commit_message>
keine Ahnung was der commit macht
</commit_message>
<xml_diff>
--- a/docs/Relationales DB Modell.xlsx
+++ b/docs/Relationales DB Modell.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Modell Fabi" sheetId="1" r:id="rId1"/>
     <sheet name="Tabellenmodell" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Modell Fabi'!$B$6:$M$24</definedName>
@@ -19,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="132">
   <si>
     <t>Relationales Datenbankmodell</t>
   </si>
@@ -270,13 +269,7 @@
     <t>VARCHAR(50)</t>
   </si>
   <si>
-    <t>ACHTUNG: VIEW!!</t>
-  </si>
-  <si>
     <t>BetAppConstantsStore</t>
-  </si>
-  <si>
-    <t>BetAppConstantsSelect</t>
   </si>
   <si>
     <t>datatype</t>
@@ -427,7 +420,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,19 +453,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,11 +478,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -637,15 +618,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -675,15 +655,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Accent3" xfId="5" builtinId="37"/>
+    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
-    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2397,14 +2375,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2279203</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>13610</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>95252</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>500742</xdr:colOff>
+      <xdr:colOff>500743</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -2415,12 +2393,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="7030135" y="5413606"/>
-          <a:ext cx="4381498" cy="602789"/>
+          <a:off x="7278463" y="5471433"/>
+          <a:ext cx="4381500" cy="487133"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 100217"/>
+            <a:gd name="adj1" fmla="val 100311"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -4200,7 +4178,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4498,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q57" sqref="Q57"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4509,7 +4487,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="33.140625" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="4.7109375" customWidth="1"/>
@@ -4525,13 +4503,13 @@
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -4551,7 +4529,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>40</v>
@@ -4569,7 +4547,7 @@
         <v>32</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Y4" s="22" t="s">
         <v>40</v>
@@ -4587,12 +4565,12 @@
         <v>32</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>33</v>
@@ -4608,7 +4586,7 @@
       </c>
       <c r="G5" s="28"/>
       <c r="N5" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>33</v>
@@ -4617,14 +4595,14 @@
         <v>55</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="S5" s="28"/>
       <c r="Y5" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Z5" s="12" t="s">
         <v>33</v>
@@ -4656,7 +4634,7 @@
       </c>
       <c r="G6" s="15"/>
       <c r="N6" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10" t="str">
@@ -4664,13 +4642,13 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>33</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>42</v>
@@ -4710,11 +4688,11 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Y7" s="5" t="s">
         <v>74</v>
@@ -4747,14 +4725,14 @@
         <v/>
       </c>
       <c r="G8" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="30" t="s">
         <v>95</v>
-      </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="31" t="s">
-        <v>97</v>
       </c>
       <c r="Q8" s="13" t="s">
         <v>39</v>
@@ -4779,12 +4757,12 @@
         <v/>
       </c>
       <c r="AD8" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="str">
@@ -4799,10 +4777,10 @@
         <v/>
       </c>
       <c r="G9" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="20" t="s">
@@ -4816,7 +4794,7 @@
       </c>
       <c r="S9" s="8"/>
       <c r="Y9" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Z9" s="10"/>
       <c r="AA9" s="13" t="s">
@@ -4828,7 +4806,7 @@
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="13" t="s">
@@ -4928,11 +4906,11 @@
       </c>
       <c r="G13" s="6"/>
       <c r="Y13" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Z13" s="10"/>
       <c r="AA13" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AB13" s="13" t="s">
         <v>39</v>
@@ -4979,7 +4957,7 @@
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
@@ -4993,11 +4971,11 @@
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>39</v>
@@ -5016,7 +4994,7 @@
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13" t="s">
@@ -5031,12 +5009,12 @@
       </c>
       <c r="G17" s="6"/>
       <c r="N17" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="str">
@@ -5051,7 +5029,7 @@
         <v/>
       </c>
       <c r="G18" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>40</v>
@@ -5069,7 +5047,7 @@
         <v>32</v>
       </c>
       <c r="S18" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
@@ -5089,7 +5067,7 @@
       </c>
       <c r="G19" s="8"/>
       <c r="N19" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>33</v>
@@ -5143,10 +5121,10 @@
         <v>33</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Y21" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
@@ -5180,12 +5158,12 @@
         <v>32</v>
       </c>
       <c r="AD22" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N23" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="20" t="s">
@@ -5213,7 +5191,7 @@
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y24" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18" t="str">
@@ -5227,7 +5205,7 @@
         <v>33</v>
       </c>
       <c r="AD24" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
@@ -5248,7 +5226,7 @@
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
@@ -5268,7 +5246,7 @@
         <v>32</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
@@ -5292,7 +5270,7 @@
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="str">
@@ -5306,10 +5284,10 @@
         <v>33</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.25">
@@ -5343,12 +5321,12 @@
         <v>32</v>
       </c>
       <c r="S32" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N33" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O33" s="10" t="s">
         <v>33</v>
@@ -5364,7 +5342,7 @@
         <v>33</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.25">
@@ -5385,10 +5363,10 @@
         <v>33</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Y34" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.25">
@@ -5422,12 +5400,12 @@
         <v>32</v>
       </c>
       <c r="AD35" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="Y36" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Z36" s="10" t="s">
         <v>33</v>
@@ -5443,7 +5421,7 @@
         <v>33</v>
       </c>
       <c r="AD36" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.25">
@@ -5464,7 +5442,7 @@
         <v>33</v>
       </c>
       <c r="AD37" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.25">
@@ -5477,16 +5455,16 @@
         <v>0</v>
       </c>
       <c r="AB38" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC38" s="11"/>
       <c r="AD38" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
@@ -5506,12 +5484,12 @@
         <v>32</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>33</v>
@@ -5527,7 +5505,7 @@
         <v>33</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
@@ -5548,7 +5526,7 @@
         <v>33</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
@@ -5565,10 +5543,10 @@
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N44" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
@@ -5588,7 +5566,7 @@
         <v>32</v>
       </c>
       <c r="S45" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
@@ -5611,7 +5589,7 @@
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N47" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O47" s="10"/>
       <c r="P47" s="10" t="s">
@@ -5625,26 +5603,26 @@
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="N48" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O48">
         <v>100</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S48" s="6"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N49" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O49" s="10"/>
       <c r="P49" s="13" t="s">
         <v>53</v>
       </c>
       <c r="Q49" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R49" s="10"/>
       <c r="S49" s="6"/>
@@ -5655,7 +5633,7 @@
       </c>
       <c r="O50" s="10"/>
       <c r="P50" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q50" s="10" t="s">
         <v>70</v>
@@ -5683,7 +5661,7 @@
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N52" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O52" s="10"/>
       <c r="P52" s="10" t="s">
@@ -5695,11 +5673,11 @@
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N53" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O53" s="10"/>
       <c r="P53" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q53" s="13" t="s">
         <v>39</v>
@@ -5711,14 +5689,14 @@
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N54" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11" t="s">
         <v>57</v>
       </c>
       <c r="Q54" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R54" s="11" t="s">
         <v>33</v>
@@ -5727,7 +5705,7 @@
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
@@ -5747,7 +5725,7 @@
         <v>32</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
@@ -5762,18 +5740,18 @@
         <v>MEDIUMINT</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>33</v>
@@ -5789,12 +5767,12 @@
         <v>33</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B71" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="2:22" x14ac:dyDescent="0.25">
@@ -5814,7 +5792,7 @@
         <v>32</v>
       </c>
       <c r="G72" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="2:22" x14ac:dyDescent="0.25">
@@ -5853,7 +5831,7 @@
     </row>
     <row r="75" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
@@ -5886,66 +5864,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>